<commit_message>
Login Positive Test is added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/registeruser.xlsx
+++ b/src/test/resources/data/registeruser.xlsx
@@ -159,9 +159,6 @@
     <t>Deli</t>
   </si>
   <si>
-    <t>ali@gmail.com</t>
-  </si>
-  <si>
     <t>12345.+</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Ali</t>
   </si>
   <si>
-    <t>a@gmail.com</t>
-  </si>
-  <si>
     <t>Last Name must be between 1 and 32 characters!</t>
   </si>
   <si>
@@ -189,13 +183,19 @@
     <t>Password confirmation does not match password!</t>
   </si>
   <si>
-    <t>ab@gmail.com</t>
-  </si>
-  <si>
-    <t>c@gmail.com</t>
-  </si>
-  <si>
-    <t>d@gmail.com</t>
+    <t>ali@ggmail.com</t>
+  </si>
+  <si>
+    <t>a@ggmail.com</t>
+  </si>
+  <si>
+    <t>ab@ggmail.com</t>
+  </si>
+  <si>
+    <t>c@ggmail.com</t>
+  </si>
+  <si>
+    <t>d@ggmail.com</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -820,19 +820,19 @@
         <v>46</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5">
         <v>5457788986</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="15.75">
@@ -840,23 +840,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E3" s="5">
         <v>5457788986</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75">
@@ -864,7 +864,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>46</v>
@@ -874,13 +874,13 @@
         <v>5457788986</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75">
@@ -888,7 +888,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>46</v>
@@ -898,13 +898,13 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="15.75">
@@ -925,10 +925,10 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="15.75">
@@ -948,11 +948,11 @@
         <v>5457788986</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +964,7 @@
     <hyperlink ref="D7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>